<commit_message>
Add new files about 1ESO and 2ESO.
</commit_message>
<xml_diff>
--- a/2022-2023/tecno1r/Exercici2.xlsx
+++ b/2022-2023/tecno1r/Exercici2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aleixjulia/Documents/GitHub/ajuliaest.github.io/2022-2023/tecno1r/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C53D3EE-3F76-AB4B-B800-FEDF660A4FE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34777547-B7DE-F446-937E-C9ECCB005664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{190AAF1F-4614-E141-8EBF-B4FF14BA4172}"/>
   </bookViews>
@@ -543,7 +543,7 @@
   <dimension ref="B1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>